<commit_message>
upper_app socket send ok, command modify, Document Maintenance
</commit_message>
<xml_diff>
--- a/document/通讯协议定义.xlsx
+++ b/document/通讯协议定义.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="242" yWindow="109" windowWidth="14799" windowHeight="8011"/>
+    <workbookView xWindow="242" yWindow="109" windowWidth="14799" windowHeight="8011" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="UART通讯协议相关" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="119">
   <si>
     <t>数据通讯</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -477,6 +477,18 @@
   </si>
   <si>
     <t>打开LED:5a 01 32 23 00 08 02 00 00 00 03 03 00 01 FF FF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>串口信息配置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">0:执行设置完毕               1:执行设置 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>网络信息配置</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -687,44 +699,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -773,15 +755,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -791,6 +764,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -800,14 +782,35 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1112,275 +1115,275 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.55" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" style="3" customWidth="1"/>
-    <col min="2" max="3" width="13.21875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="19.109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="13" style="3" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="14.77734375" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="19.77734375" style="2" customWidth="1"/>
+    <col min="2" max="3" width="13.21875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.77734375" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-    </row>
-    <row r="4" spans="1:7" s="15" customFormat="1" ht="29.05" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" s="5" customFormat="1" ht="29.05" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="15" customFormat="1" ht="29.05" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:7" s="5" customFormat="1" ht="29.05" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="29.05" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="16"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:7" ht="14.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="16"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:7" ht="14.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="D10" s="28"/>
-      <c r="E10" s="16"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:7" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="16"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="16"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:7" ht="14.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="16"/>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="25"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="15"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G15" s="2">
+      <c r="G15" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-    </row>
-    <row r="19" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+    </row>
+    <row r="19" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-    </row>
-    <row r="20" spans="1:7" s="15" customFormat="1" ht="29.05" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:7" s="5" customFormat="1" ht="29.05" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="G20" s="13" t="s">
+      <c r="G20" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="15" customFormat="1" ht="29.05" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+    <row r="21" spans="1:7" s="5" customFormat="1" ht="29.05" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F21" s="13" t="s">
+      <c r="F21" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G21" s="13" t="s">
+      <c r="G21" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1404,287 +1407,301 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.55" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18.21875" style="1" customWidth="1"/>
-    <col min="3" max="5" width="8.88671875" style="1"/>
-    <col min="6" max="6" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.21875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.88671875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="2" width="18.21875" style="28" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="28"/>
+    <col min="4" max="4" width="21.5546875" style="28" customWidth="1"/>
+    <col min="5" max="5" width="20.109375" style="28" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="28" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" style="28" customWidth="1"/>
+    <col min="8" max="8" width="18.21875" style="28" customWidth="1"/>
+    <col min="9" max="9" width="21.88671875" style="28" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="28"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="28" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="28" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.15" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:9" ht="16.350000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="32"/>
     </row>
     <row r="6" spans="1:9" ht="16.350000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="7">
+      <c r="A6" s="33"/>
+      <c r="B6" s="34">
         <v>7</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="34">
         <v>6</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="34">
         <v>5</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="34">
         <v>4</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="35">
         <v>3</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="34">
         <v>2</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="34">
         <v>1</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="34">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="16.350000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="23" t="s">
+      <c r="C7" s="21"/>
+      <c r="D7" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="E7" s="37" t="s">
+        <v>116</v>
+      </c>
+      <c r="F7" s="37" t="s">
         <v>113</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="37" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="32.1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:9" ht="56.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="23" t="s">
+      <c r="C8" s="21"/>
+      <c r="D8" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="E8" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="F8" s="37" t="s">
         <v>114</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="37" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.15" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:9" ht="16.350000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="32"/>
     </row>
     <row r="11" spans="1:9" ht="16.350000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="8">
+      <c r="A11" s="33"/>
+      <c r="B11" s="34">
         <v>7</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="34">
         <v>6</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="34">
         <v>5</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="34">
         <v>4</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="34">
         <v>3</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="34">
         <v>2</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="34">
         <v>1</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11" s="34">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="16.350000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="34"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="21"/>
     </row>
     <row r="13" spans="1:9" ht="16.350000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="34"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="21"/>
     </row>
     <row r="15" spans="1:9" ht="15.15" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:9" ht="16.350000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="32"/>
     </row>
     <row r="17" spans="1:9" ht="16.350000000000001" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="7">
+      <c r="A17" s="33"/>
+      <c r="B17" s="34">
         <v>7</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="34">
         <v>6</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="34">
         <v>5</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="34">
         <v>4</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="34">
         <v>3</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="34">
         <v>2</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H17" s="34">
         <v>1</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="34">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="25.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8" t="s">
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="I18" s="8" t="s">
+      <c r="I18" s="34" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8" t="s">
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="I19" s="8" t="s">
+      <c r="I19" s="34" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="9">
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
     <mergeCell ref="B5:I5"/>
     <mergeCell ref="B16:I16"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B12:I12"/>
     <mergeCell ref="B13:I13"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1702,1190 +1719,1186 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="18.21875" style="19" customWidth="1"/>
-    <col min="3" max="5" width="8.88671875" style="19"/>
-    <col min="6" max="6" width="15.6640625" style="19" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" style="19" customWidth="1"/>
-    <col min="8" max="8" width="18.21875" style="19" customWidth="1"/>
-    <col min="9" max="9" width="21.88671875" style="19" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="19"/>
+    <col min="1" max="2" width="18.21875" style="9" customWidth="1"/>
+    <col min="3" max="5" width="8.88671875" style="9"/>
+    <col min="6" max="6" width="15.6640625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="18.21875" style="9" customWidth="1"/>
+    <col min="9" max="9" width="21.88671875" style="9" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="37"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="27"/>
     </row>
     <row r="3" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="21"/>
-      <c r="B3" s="17">
+      <c r="A3" s="11"/>
+      <c r="B3" s="7">
         <v>7</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="7">
         <v>6</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="7">
         <v>5</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="7">
         <v>4</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="7">
         <v>3</v>
       </c>
-      <c r="G3" s="17">
+      <c r="G3" s="7">
         <v>2</v>
       </c>
-      <c r="H3" s="17">
+      <c r="H3" s="7">
         <v>1</v>
       </c>
-      <c r="I3" s="17">
+      <c r="I3" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="18" customFormat="1" ht="21.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
+    <row r="4" spans="1:9" s="8" customFormat="1" ht="21.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="23" t="s">
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="I4" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="18" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="21" t="s">
+    <row r="5" spans="1:9" s="8" customFormat="1" ht="29.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="17" t="s">
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="I5" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="37"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="27"/>
     </row>
     <row r="9" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="21"/>
-      <c r="B9" s="17">
+      <c r="A9" s="11"/>
+      <c r="B9" s="7">
         <v>7</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="7">
         <v>6</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="7">
         <v>5</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="7">
         <v>4</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="7">
         <v>3</v>
       </c>
-      <c r="G9" s="17">
+      <c r="G9" s="7">
         <v>2</v>
       </c>
-      <c r="H9" s="17">
+      <c r="H9" s="7">
         <v>1</v>
       </c>
-      <c r="I9" s="17">
+      <c r="I9" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="21.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="40"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="24"/>
     </row>
     <row r="11" spans="1:9" ht="27.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="40"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="24"/>
     </row>
     <row r="13" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="37"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="27"/>
     </row>
     <row r="15" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="21"/>
-      <c r="B15" s="17">
+      <c r="A15" s="11"/>
+      <c r="B15" s="7">
         <v>7</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C15" s="7">
         <v>6</v>
       </c>
-      <c r="D15" s="17">
+      <c r="D15" s="7">
         <v>5</v>
       </c>
-      <c r="E15" s="17">
+      <c r="E15" s="7">
         <v>4</v>
       </c>
-      <c r="F15" s="17">
+      <c r="F15" s="7">
         <v>3</v>
       </c>
-      <c r="G15" s="17">
+      <c r="G15" s="7">
         <v>2</v>
       </c>
-      <c r="H15" s="17">
+      <c r="H15" s="7">
         <v>1</v>
       </c>
-      <c r="I15" s="17">
+      <c r="I15" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="40"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="24"/>
     </row>
     <row r="17" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="38"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="40"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="24"/>
     </row>
     <row r="19" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="20" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="37"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="27"/>
     </row>
     <row r="21" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="21"/>
-      <c r="B21" s="17">
+      <c r="A21" s="11"/>
+      <c r="B21" s="7">
         <v>7</v>
       </c>
-      <c r="C21" s="17">
+      <c r="C21" s="7">
         <v>6</v>
       </c>
-      <c r="D21" s="17">
+      <c r="D21" s="7">
         <v>5</v>
       </c>
-      <c r="E21" s="17">
+      <c r="E21" s="7">
         <v>4</v>
       </c>
-      <c r="F21" s="17">
+      <c r="F21" s="7">
         <v>3</v>
       </c>
-      <c r="G21" s="17">
+      <c r="G21" s="7">
         <v>2</v>
       </c>
-      <c r="H21" s="17">
+      <c r="H21" s="7">
         <v>1</v>
       </c>
-      <c r="I21" s="17">
+      <c r="I21" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="11.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="38" t="s">
+      <c r="B22" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="40"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="24"/>
     </row>
     <row r="23" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="38"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="40"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="24"/>
     </row>
     <row r="25" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="26" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B26" s="35" t="s">
+      <c r="B26" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="37"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="27"/>
     </row>
     <row r="27" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="21"/>
-      <c r="B27" s="17">
+      <c r="A27" s="11"/>
+      <c r="B27" s="7">
         <v>7</v>
       </c>
-      <c r="C27" s="17">
+      <c r="C27" s="7">
         <v>6</v>
       </c>
-      <c r="D27" s="17">
+      <c r="D27" s="7">
         <v>5</v>
       </c>
-      <c r="E27" s="17">
+      <c r="E27" s="7">
         <v>4</v>
       </c>
-      <c r="F27" s="17">
+      <c r="F27" s="7">
         <v>3</v>
       </c>
-      <c r="G27" s="17">
+      <c r="G27" s="7">
         <v>2</v>
       </c>
-      <c r="H27" s="17">
+      <c r="H27" s="7">
         <v>1</v>
       </c>
-      <c r="I27" s="17">
+      <c r="I27" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="21" t="s">
+      <c r="A28" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="38" t="s">
+      <c r="B28" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="40"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="24"/>
     </row>
     <row r="29" spans="1:9" ht="11.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="21" t="s">
+      <c r="A29" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="40"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="24"/>
     </row>
     <row r="30" spans="1:9" ht="11.95" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="31" spans="1:9" ht="11.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="32" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="20" t="s">
+      <c r="A32" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="B32" s="35" t="s">
+      <c r="B32" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="37"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="27"/>
     </row>
     <row r="33" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="21"/>
-      <c r="B33" s="17">
+      <c r="A33" s="11"/>
+      <c r="B33" s="7">
         <v>7</v>
       </c>
-      <c r="C33" s="17">
+      <c r="C33" s="7">
         <v>6</v>
       </c>
-      <c r="D33" s="17">
+      <c r="D33" s="7">
         <v>5</v>
       </c>
-      <c r="E33" s="17">
+      <c r="E33" s="7">
         <v>4</v>
       </c>
-      <c r="F33" s="17">
+      <c r="F33" s="7">
         <v>3</v>
       </c>
-      <c r="G33" s="17">
+      <c r="G33" s="7">
         <v>2</v>
       </c>
-      <c r="H33" s="17">
+      <c r="H33" s="7">
         <v>1</v>
       </c>
-      <c r="I33" s="17">
+      <c r="I33" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="21" t="s">
+      <c r="A34" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="38" t="s">
+      <c r="B34" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="C34" s="39"/>
-      <c r="D34" s="39"/>
-      <c r="E34" s="39"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="39"/>
-      <c r="H34" s="39"/>
-      <c r="I34" s="40"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="24"/>
     </row>
     <row r="35" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="21" t="s">
+      <c r="A35" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B35" s="38" t="s">
+      <c r="B35" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="39"/>
-      <c r="D35" s="39"/>
-      <c r="E35" s="39"/>
-      <c r="F35" s="39"/>
-      <c r="G35" s="39"/>
-      <c r="H35" s="39"/>
-      <c r="I35" s="40"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="24"/>
     </row>
     <row r="37" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="20" t="s">
+      <c r="A38" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="B38" s="35" t="s">
+      <c r="B38" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="37"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="27"/>
     </row>
     <row r="39" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="21"/>
-      <c r="B39" s="17">
+      <c r="A39" s="11"/>
+      <c r="B39" s="7">
         <v>7</v>
       </c>
-      <c r="C39" s="17">
+      <c r="C39" s="7">
         <v>6</v>
       </c>
-      <c r="D39" s="17">
+      <c r="D39" s="7">
         <v>5</v>
       </c>
-      <c r="E39" s="17">
+      <c r="E39" s="7">
         <v>4</v>
       </c>
-      <c r="F39" s="17">
+      <c r="F39" s="7">
         <v>3</v>
       </c>
-      <c r="G39" s="17">
+      <c r="G39" s="7">
         <v>2</v>
       </c>
-      <c r="H39" s="17">
+      <c r="H39" s="7">
         <v>1</v>
       </c>
-      <c r="I39" s="17">
+      <c r="I39" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="21" t="s">
+      <c r="A40" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B40" s="38"/>
-      <c r="C40" s="39"/>
-      <c r="D40" s="39"/>
-      <c r="E40" s="39"/>
-      <c r="F40" s="39"/>
-      <c r="G40" s="39"/>
-      <c r="H40" s="39"/>
-      <c r="I40" s="40"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="23"/>
+      <c r="H40" s="23"/>
+      <c r="I40" s="24"/>
     </row>
     <row r="41" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="21" t="s">
+      <c r="A41" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B41" s="38"/>
-      <c r="C41" s="39"/>
-      <c r="D41" s="39"/>
-      <c r="E41" s="39"/>
-      <c r="F41" s="39"/>
-      <c r="G41" s="39"/>
-      <c r="H41" s="39"/>
-      <c r="I41" s="40"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="23"/>
+      <c r="G41" s="23"/>
+      <c r="H41" s="23"/>
+      <c r="I41" s="24"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B42" s="22"/>
-      <c r="C42" s="22"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="22"/>
-      <c r="G42" s="22"/>
-      <c r="H42" s="22"/>
-      <c r="I42" s="22"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="12"/>
     </row>
     <row r="43" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="44" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="20" t="s">
+      <c r="A44" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="B44" s="35" t="s">
+      <c r="B44" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C44" s="36"/>
-      <c r="D44" s="36"/>
-      <c r="E44" s="36"/>
-      <c r="F44" s="36"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="37"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="26"/>
+      <c r="G44" s="26"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="27"/>
     </row>
     <row r="45" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="21"/>
-      <c r="B45" s="17">
+      <c r="A45" s="11"/>
+      <c r="B45" s="7">
         <v>7</v>
       </c>
-      <c r="C45" s="17">
+      <c r="C45" s="7">
         <v>6</v>
       </c>
-      <c r="D45" s="17">
+      <c r="D45" s="7">
         <v>5</v>
       </c>
-      <c r="E45" s="17">
+      <c r="E45" s="7">
         <v>4</v>
       </c>
-      <c r="F45" s="17">
+      <c r="F45" s="7">
         <v>3</v>
       </c>
-      <c r="G45" s="17">
+      <c r="G45" s="7">
         <v>2</v>
       </c>
-      <c r="H45" s="17">
+      <c r="H45" s="7">
         <v>1</v>
       </c>
-      <c r="I45" s="17">
+      <c r="I45" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="21" t="s">
+      <c r="A46" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B46" s="38"/>
-      <c r="C46" s="39"/>
-      <c r="D46" s="39"/>
-      <c r="E46" s="39"/>
-      <c r="F46" s="39"/>
-      <c r="G46" s="39"/>
-      <c r="H46" s="39"/>
-      <c r="I46" s="40"/>
+      <c r="B46" s="22"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="23"/>
+      <c r="F46" s="23"/>
+      <c r="G46" s="23"/>
+      <c r="H46" s="23"/>
+      <c r="I46" s="24"/>
     </row>
     <row r="47" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="21" t="s">
+      <c r="A47" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B47" s="38"/>
-      <c r="C47" s="39"/>
-      <c r="D47" s="39"/>
-      <c r="E47" s="39"/>
-      <c r="F47" s="39"/>
-      <c r="G47" s="39"/>
-      <c r="H47" s="39"/>
-      <c r="I47" s="40"/>
+      <c r="B47" s="22"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="23"/>
+      <c r="F47" s="23"/>
+      <c r="G47" s="23"/>
+      <c r="H47" s="23"/>
+      <c r="I47" s="24"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B48" s="22"/>
-      <c r="C48" s="22"/>
-      <c r="D48" s="22"/>
-      <c r="E48" s="22"/>
-      <c r="F48" s="22"/>
-      <c r="G48" s="22"/>
-      <c r="H48" s="22"/>
-      <c r="I48" s="22"/>
+      <c r="B48" s="12"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="12"/>
+      <c r="I48" s="12"/>
     </row>
     <row r="49" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="50" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="20" t="s">
+      <c r="A50" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="B50" s="35" t="s">
+      <c r="B50" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="C50" s="36"/>
-      <c r="D50" s="36"/>
-      <c r="E50" s="36"/>
-      <c r="F50" s="36"/>
-      <c r="G50" s="36"/>
-      <c r="H50" s="36"/>
-      <c r="I50" s="37"/>
+      <c r="C50" s="26"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="26"/>
+      <c r="F50" s="26"/>
+      <c r="G50" s="26"/>
+      <c r="H50" s="26"/>
+      <c r="I50" s="27"/>
     </row>
     <row r="51" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="21"/>
-      <c r="B51" s="17">
+      <c r="A51" s="11"/>
+      <c r="B51" s="7">
         <v>7</v>
       </c>
-      <c r="C51" s="17">
+      <c r="C51" s="7">
         <v>6</v>
       </c>
-      <c r="D51" s="17">
+      <c r="D51" s="7">
         <v>5</v>
       </c>
-      <c r="E51" s="17">
+      <c r="E51" s="7">
         <v>4</v>
       </c>
-      <c r="F51" s="17">
+      <c r="F51" s="7">
         <v>3</v>
       </c>
-      <c r="G51" s="17">
+      <c r="G51" s="7">
         <v>2</v>
       </c>
-      <c r="H51" s="17">
+      <c r="H51" s="7">
         <v>1</v>
       </c>
-      <c r="I51" s="17">
+      <c r="I51" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="21" t="s">
+      <c r="A52" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B52" s="38"/>
-      <c r="C52" s="39"/>
-      <c r="D52" s="39"/>
-      <c r="E52" s="39"/>
-      <c r="F52" s="39"/>
-      <c r="G52" s="39"/>
-      <c r="H52" s="39"/>
-      <c r="I52" s="40"/>
+      <c r="B52" s="22"/>
+      <c r="C52" s="23"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="23"/>
+      <c r="F52" s="23"/>
+      <c r="G52" s="23"/>
+      <c r="H52" s="23"/>
+      <c r="I52" s="24"/>
     </row>
     <row r="53" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="21" t="s">
+      <c r="A53" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B53" s="38"/>
-      <c r="C53" s="39"/>
-      <c r="D53" s="39"/>
-      <c r="E53" s="39"/>
-      <c r="F53" s="39"/>
-      <c r="G53" s="39"/>
-      <c r="H53" s="39"/>
-      <c r="I53" s="40"/>
+      <c r="B53" s="22"/>
+      <c r="C53" s="23"/>
+      <c r="D53" s="23"/>
+      <c r="E53" s="23"/>
+      <c r="F53" s="23"/>
+      <c r="G53" s="23"/>
+      <c r="H53" s="23"/>
+      <c r="I53" s="24"/>
     </row>
     <row r="55" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="56" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="20" t="s">
+      <c r="A56" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="B56" s="35" t="s">
+      <c r="B56" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C56" s="36"/>
-      <c r="D56" s="36"/>
-      <c r="E56" s="36"/>
-      <c r="F56" s="36"/>
-      <c r="G56" s="36"/>
-      <c r="H56" s="36"/>
-      <c r="I56" s="37"/>
+      <c r="C56" s="26"/>
+      <c r="D56" s="26"/>
+      <c r="E56" s="26"/>
+      <c r="F56" s="26"/>
+      <c r="G56" s="26"/>
+      <c r="H56" s="26"/>
+      <c r="I56" s="27"/>
     </row>
     <row r="57" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="21"/>
-      <c r="B57" s="17">
+      <c r="A57" s="11"/>
+      <c r="B57" s="7">
         <v>7</v>
       </c>
-      <c r="C57" s="17">
+      <c r="C57" s="7">
         <v>6</v>
       </c>
-      <c r="D57" s="17">
+      <c r="D57" s="7">
         <v>5</v>
       </c>
-      <c r="E57" s="17">
+      <c r="E57" s="7">
         <v>4</v>
       </c>
-      <c r="F57" s="17">
+      <c r="F57" s="7">
         <v>3</v>
       </c>
-      <c r="G57" s="17">
+      <c r="G57" s="7">
         <v>2</v>
       </c>
-      <c r="H57" s="17">
+      <c r="H57" s="7">
         <v>1</v>
       </c>
-      <c r="I57" s="17">
+      <c r="I57" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="21" t="s">
+      <c r="A58" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B58" s="38"/>
-      <c r="C58" s="39"/>
-      <c r="D58" s="39"/>
-      <c r="E58" s="39"/>
-      <c r="F58" s="39"/>
-      <c r="G58" s="39"/>
-      <c r="H58" s="39"/>
-      <c r="I58" s="40"/>
+      <c r="B58" s="22"/>
+      <c r="C58" s="23"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="23"/>
+      <c r="F58" s="23"/>
+      <c r="G58" s="23"/>
+      <c r="H58" s="23"/>
+      <c r="I58" s="24"/>
     </row>
     <row r="59" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="21" t="s">
+      <c r="A59" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B59" s="38"/>
-      <c r="C59" s="39"/>
-      <c r="D59" s="39"/>
-      <c r="E59" s="39"/>
-      <c r="F59" s="39"/>
-      <c r="G59" s="39"/>
-      <c r="H59" s="39"/>
-      <c r="I59" s="40"/>
+      <c r="B59" s="22"/>
+      <c r="C59" s="23"/>
+      <c r="D59" s="23"/>
+      <c r="E59" s="23"/>
+      <c r="F59" s="23"/>
+      <c r="G59" s="23"/>
+      <c r="H59" s="23"/>
+      <c r="I59" s="24"/>
     </row>
     <row r="61" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="62" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="20" t="s">
+      <c r="A62" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="B62" s="35" t="s">
+      <c r="B62" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="C62" s="36"/>
-      <c r="D62" s="36"/>
-      <c r="E62" s="36"/>
-      <c r="F62" s="36"/>
-      <c r="G62" s="36"/>
-      <c r="H62" s="36"/>
-      <c r="I62" s="37"/>
+      <c r="C62" s="26"/>
+      <c r="D62" s="26"/>
+      <c r="E62" s="26"/>
+      <c r="F62" s="26"/>
+      <c r="G62" s="26"/>
+      <c r="H62" s="26"/>
+      <c r="I62" s="27"/>
     </row>
     <row r="63" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="21"/>
-      <c r="B63" s="17">
+      <c r="A63" s="11"/>
+      <c r="B63" s="7">
         <v>7</v>
       </c>
-      <c r="C63" s="17">
+      <c r="C63" s="7">
         <v>6</v>
       </c>
-      <c r="D63" s="17">
+      <c r="D63" s="7">
         <v>5</v>
       </c>
-      <c r="E63" s="17">
+      <c r="E63" s="7">
         <v>4</v>
       </c>
-      <c r="F63" s="17">
+      <c r="F63" s="7">
         <v>3</v>
       </c>
-      <c r="G63" s="17">
+      <c r="G63" s="7">
         <v>2</v>
       </c>
-      <c r="H63" s="17">
+      <c r="H63" s="7">
         <v>1</v>
       </c>
-      <c r="I63" s="17">
+      <c r="I63" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="21" t="s">
+      <c r="A64" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B64" s="38"/>
-      <c r="C64" s="39"/>
-      <c r="D64" s="39"/>
-      <c r="E64" s="39"/>
-      <c r="F64" s="39"/>
-      <c r="G64" s="39"/>
-      <c r="H64" s="39"/>
-      <c r="I64" s="40"/>
+      <c r="B64" s="22"/>
+      <c r="C64" s="23"/>
+      <c r="D64" s="23"/>
+      <c r="E64" s="23"/>
+      <c r="F64" s="23"/>
+      <c r="G64" s="23"/>
+      <c r="H64" s="23"/>
+      <c r="I64" s="24"/>
     </row>
     <row r="65" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="21" t="s">
+      <c r="A65" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B65" s="38"/>
-      <c r="C65" s="39"/>
-      <c r="D65" s="39"/>
-      <c r="E65" s="39"/>
-      <c r="F65" s="39"/>
-      <c r="G65" s="39"/>
-      <c r="H65" s="39"/>
-      <c r="I65" s="40"/>
+      <c r="B65" s="22"/>
+      <c r="C65" s="23"/>
+      <c r="D65" s="23"/>
+      <c r="E65" s="23"/>
+      <c r="F65" s="23"/>
+      <c r="G65" s="23"/>
+      <c r="H65" s="23"/>
+      <c r="I65" s="24"/>
     </row>
     <row r="67" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="68" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="20" t="s">
+      <c r="A68" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="B68" s="35" t="s">
+      <c r="B68" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="C68" s="36"/>
-      <c r="D68" s="36"/>
-      <c r="E68" s="36"/>
-      <c r="F68" s="36"/>
-      <c r="G68" s="36"/>
-      <c r="H68" s="36"/>
-      <c r="I68" s="37"/>
+      <c r="C68" s="26"/>
+      <c r="D68" s="26"/>
+      <c r="E68" s="26"/>
+      <c r="F68" s="26"/>
+      <c r="G68" s="26"/>
+      <c r="H68" s="26"/>
+      <c r="I68" s="27"/>
     </row>
     <row r="69" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="21"/>
-      <c r="B69" s="17">
+      <c r="A69" s="11"/>
+      <c r="B69" s="7">
         <v>7</v>
       </c>
-      <c r="C69" s="17">
+      <c r="C69" s="7">
         <v>6</v>
       </c>
-      <c r="D69" s="17">
+      <c r="D69" s="7">
         <v>5</v>
       </c>
-      <c r="E69" s="17">
+      <c r="E69" s="7">
         <v>4</v>
       </c>
-      <c r="F69" s="17">
+      <c r="F69" s="7">
         <v>3</v>
       </c>
-      <c r="G69" s="17">
+      <c r="G69" s="7">
         <v>2</v>
       </c>
-      <c r="H69" s="17">
+      <c r="H69" s="7">
         <v>1</v>
       </c>
-      <c r="I69" s="17">
+      <c r="I69" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="21" t="s">
+      <c r="A70" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B70" s="38"/>
-      <c r="C70" s="39"/>
-      <c r="D70" s="39"/>
-      <c r="E70" s="39"/>
-      <c r="F70" s="39"/>
-      <c r="G70" s="39"/>
-      <c r="H70" s="39"/>
-      <c r="I70" s="40"/>
+      <c r="B70" s="22"/>
+      <c r="C70" s="23"/>
+      <c r="D70" s="23"/>
+      <c r="E70" s="23"/>
+      <c r="F70" s="23"/>
+      <c r="G70" s="23"/>
+      <c r="H70" s="23"/>
+      <c r="I70" s="24"/>
     </row>
     <row r="71" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="21" t="s">
+      <c r="A71" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B71" s="38"/>
-      <c r="C71" s="39"/>
-      <c r="D71" s="39"/>
-      <c r="E71" s="39"/>
-      <c r="F71" s="39"/>
-      <c r="G71" s="39"/>
-      <c r="H71" s="39"/>
-      <c r="I71" s="40"/>
+      <c r="B71" s="22"/>
+      <c r="C71" s="23"/>
+      <c r="D71" s="23"/>
+      <c r="E71" s="23"/>
+      <c r="F71" s="23"/>
+      <c r="G71" s="23"/>
+      <c r="H71" s="23"/>
+      <c r="I71" s="24"/>
     </row>
     <row r="73" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="74" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="20" t="s">
+      <c r="A74" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="B74" s="35" t="s">
+      <c r="B74" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C74" s="36"/>
-      <c r="D74" s="36"/>
-      <c r="E74" s="36"/>
-      <c r="F74" s="36"/>
-      <c r="G74" s="36"/>
-      <c r="H74" s="36"/>
-      <c r="I74" s="37"/>
+      <c r="C74" s="26"/>
+      <c r="D74" s="26"/>
+      <c r="E74" s="26"/>
+      <c r="F74" s="26"/>
+      <c r="G74" s="26"/>
+      <c r="H74" s="26"/>
+      <c r="I74" s="27"/>
     </row>
     <row r="75" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="21"/>
-      <c r="B75" s="17">
+      <c r="A75" s="11"/>
+      <c r="B75" s="7">
         <v>7</v>
       </c>
-      <c r="C75" s="17">
+      <c r="C75" s="7">
         <v>6</v>
       </c>
-      <c r="D75" s="17">
+      <c r="D75" s="7">
         <v>5</v>
       </c>
-      <c r="E75" s="17">
+      <c r="E75" s="7">
         <v>4</v>
       </c>
-      <c r="F75" s="17">
+      <c r="F75" s="7">
         <v>3</v>
       </c>
-      <c r="G75" s="17">
+      <c r="G75" s="7">
         <v>2</v>
       </c>
-      <c r="H75" s="17">
+      <c r="H75" s="7">
         <v>1</v>
       </c>
-      <c r="I75" s="17">
+      <c r="I75" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="21" t="s">
+      <c r="A76" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B76" s="38"/>
-      <c r="C76" s="39"/>
-      <c r="D76" s="39"/>
-      <c r="E76" s="39"/>
-      <c r="F76" s="39"/>
-      <c r="G76" s="39"/>
-      <c r="H76" s="39"/>
-      <c r="I76" s="40"/>
+      <c r="B76" s="22"/>
+      <c r="C76" s="23"/>
+      <c r="D76" s="23"/>
+      <c r="E76" s="23"/>
+      <c r="F76" s="23"/>
+      <c r="G76" s="23"/>
+      <c r="H76" s="23"/>
+      <c r="I76" s="24"/>
     </row>
     <row r="77" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="21" t="s">
+      <c r="A77" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B77" s="38"/>
-      <c r="C77" s="39"/>
-      <c r="D77" s="39"/>
-      <c r="E77" s="39"/>
-      <c r="F77" s="39"/>
-      <c r="G77" s="39"/>
-      <c r="H77" s="39"/>
-      <c r="I77" s="40"/>
+      <c r="B77" s="22"/>
+      <c r="C77" s="23"/>
+      <c r="D77" s="23"/>
+      <c r="E77" s="23"/>
+      <c r="F77" s="23"/>
+      <c r="G77" s="23"/>
+      <c r="H77" s="23"/>
+      <c r="I77" s="24"/>
     </row>
     <row r="79" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="80" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="20" t="s">
+      <c r="A80" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="B80" s="35" t="s">
+      <c r="B80" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="C80" s="36"/>
-      <c r="D80" s="36"/>
-      <c r="E80" s="36"/>
-      <c r="F80" s="36"/>
-      <c r="G80" s="36"/>
-      <c r="H80" s="36"/>
-      <c r="I80" s="37"/>
+      <c r="C80" s="26"/>
+      <c r="D80" s="26"/>
+      <c r="E80" s="26"/>
+      <c r="F80" s="26"/>
+      <c r="G80" s="26"/>
+      <c r="H80" s="26"/>
+      <c r="I80" s="27"/>
     </row>
     <row r="81" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="21"/>
-      <c r="B81" s="17">
+      <c r="A81" s="11"/>
+      <c r="B81" s="7">
         <v>7</v>
       </c>
-      <c r="C81" s="17">
+      <c r="C81" s="7">
         <v>6</v>
       </c>
-      <c r="D81" s="17">
+      <c r="D81" s="7">
         <v>5</v>
       </c>
-      <c r="E81" s="17">
+      <c r="E81" s="7">
         <v>4</v>
       </c>
-      <c r="F81" s="17">
+      <c r="F81" s="7">
         <v>3</v>
       </c>
-      <c r="G81" s="17">
+      <c r="G81" s="7">
         <v>2</v>
       </c>
-      <c r="H81" s="17">
+      <c r="H81" s="7">
         <v>1</v>
       </c>
-      <c r="I81" s="17">
+      <c r="I81" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="21" t="s">
+      <c r="A82" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B82" s="38"/>
-      <c r="C82" s="39"/>
-      <c r="D82" s="39"/>
-      <c r="E82" s="39"/>
-      <c r="F82" s="39"/>
-      <c r="G82" s="39"/>
-      <c r="H82" s="39"/>
-      <c r="I82" s="40"/>
+      <c r="B82" s="22"/>
+      <c r="C82" s="23"/>
+      <c r="D82" s="23"/>
+      <c r="E82" s="23"/>
+      <c r="F82" s="23"/>
+      <c r="G82" s="23"/>
+      <c r="H82" s="23"/>
+      <c r="I82" s="24"/>
     </row>
     <row r="83" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="21" t="s">
+      <c r="A83" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B83" s="38"/>
-      <c r="C83" s="39"/>
-      <c r="D83" s="39"/>
-      <c r="E83" s="39"/>
-      <c r="F83" s="39"/>
-      <c r="G83" s="39"/>
-      <c r="H83" s="39"/>
-      <c r="I83" s="40"/>
+      <c r="B83" s="22"/>
+      <c r="C83" s="23"/>
+      <c r="D83" s="23"/>
+      <c r="E83" s="23"/>
+      <c r="F83" s="23"/>
+      <c r="G83" s="23"/>
+      <c r="H83" s="23"/>
+      <c r="I83" s="24"/>
     </row>
     <row r="85" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="86" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="20" t="s">
+      <c r="A86" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="B86" s="35" t="s">
+      <c r="B86" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="C86" s="36"/>
-      <c r="D86" s="36"/>
-      <c r="E86" s="36"/>
-      <c r="F86" s="36"/>
-      <c r="G86" s="36"/>
-      <c r="H86" s="36"/>
-      <c r="I86" s="37"/>
+      <c r="C86" s="26"/>
+      <c r="D86" s="26"/>
+      <c r="E86" s="26"/>
+      <c r="F86" s="26"/>
+      <c r="G86" s="26"/>
+      <c r="H86" s="26"/>
+      <c r="I86" s="27"/>
     </row>
     <row r="87" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="21"/>
-      <c r="B87" s="17">
+      <c r="A87" s="11"/>
+      <c r="B87" s="7">
         <v>7</v>
       </c>
-      <c r="C87" s="17">
+      <c r="C87" s="7">
         <v>6</v>
       </c>
-      <c r="D87" s="17">
+      <c r="D87" s="7">
         <v>5</v>
       </c>
-      <c r="E87" s="17">
+      <c r="E87" s="7">
         <v>4</v>
       </c>
-      <c r="F87" s="17">
+      <c r="F87" s="7">
         <v>3</v>
       </c>
-      <c r="G87" s="17">
+      <c r="G87" s="7">
         <v>2</v>
       </c>
-      <c r="H87" s="17">
+      <c r="H87" s="7">
         <v>1</v>
       </c>
-      <c r="I87" s="17">
+      <c r="I87" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="21" t="s">
+      <c r="A88" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B88" s="38"/>
-      <c r="C88" s="39"/>
-      <c r="D88" s="39"/>
-      <c r="E88" s="39"/>
-      <c r="F88" s="39"/>
-      <c r="G88" s="39"/>
-      <c r="H88" s="39"/>
-      <c r="I88" s="40"/>
+      <c r="B88" s="22"/>
+      <c r="C88" s="23"/>
+      <c r="D88" s="23"/>
+      <c r="E88" s="23"/>
+      <c r="F88" s="23"/>
+      <c r="G88" s="23"/>
+      <c r="H88" s="23"/>
+      <c r="I88" s="24"/>
     </row>
     <row r="89" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="21" t="s">
+      <c r="A89" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B89" s="38"/>
-      <c r="C89" s="39"/>
-      <c r="D89" s="39"/>
-      <c r="E89" s="39"/>
-      <c r="F89" s="39"/>
-      <c r="G89" s="39"/>
-      <c r="H89" s="39"/>
-      <c r="I89" s="40"/>
+      <c r="B89" s="22"/>
+      <c r="C89" s="23"/>
+      <c r="D89" s="23"/>
+      <c r="E89" s="23"/>
+      <c r="F89" s="23"/>
+      <c r="G89" s="23"/>
+      <c r="H89" s="23"/>
+      <c r="I89" s="24"/>
     </row>
     <row r="91" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="92" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="20" t="s">
+      <c r="A92" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="B92" s="35" t="s">
+      <c r="B92" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="C92" s="36"/>
-      <c r="D92" s="36"/>
-      <c r="E92" s="36"/>
-      <c r="F92" s="36"/>
-      <c r="G92" s="36"/>
-      <c r="H92" s="36"/>
-      <c r="I92" s="37"/>
+      <c r="C92" s="26"/>
+      <c r="D92" s="26"/>
+      <c r="E92" s="26"/>
+      <c r="F92" s="26"/>
+      <c r="G92" s="26"/>
+      <c r="H92" s="26"/>
+      <c r="I92" s="27"/>
     </row>
     <row r="93" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="21"/>
-      <c r="B93" s="17">
+      <c r="A93" s="11"/>
+      <c r="B93" s="7">
         <v>7</v>
       </c>
-      <c r="C93" s="17">
+      <c r="C93" s="7">
         <v>6</v>
       </c>
-      <c r="D93" s="17">
+      <c r="D93" s="7">
         <v>5</v>
       </c>
-      <c r="E93" s="17">
+      <c r="E93" s="7">
         <v>4</v>
       </c>
-      <c r="F93" s="17">
+      <c r="F93" s="7">
         <v>3</v>
       </c>
-      <c r="G93" s="17">
+      <c r="G93" s="7">
         <v>2</v>
       </c>
-      <c r="H93" s="17">
+      <c r="H93" s="7">
         <v>1</v>
       </c>
-      <c r="I93" s="17">
+      <c r="I93" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="21" t="s">
+      <c r="A94" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B94" s="38" t="s">
+      <c r="B94" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="C94" s="39"/>
-      <c r="D94" s="39"/>
-      <c r="E94" s="39"/>
-      <c r="F94" s="39"/>
-      <c r="G94" s="39"/>
-      <c r="H94" s="39"/>
-      <c r="I94" s="40"/>
+      <c r="C94" s="23"/>
+      <c r="D94" s="23"/>
+      <c r="E94" s="23"/>
+      <c r="F94" s="23"/>
+      <c r="G94" s="23"/>
+      <c r="H94" s="23"/>
+      <c r="I94" s="24"/>
     </row>
     <row r="95" spans="1:9" ht="12.7" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="21" t="s">
+      <c r="A95" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B95" s="38" t="s">
+      <c r="B95" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C95" s="39"/>
-      <c r="D95" s="39"/>
-      <c r="E95" s="39"/>
-      <c r="F95" s="39"/>
-      <c r="G95" s="39"/>
-      <c r="H95" s="39"/>
-      <c r="I95" s="40"/>
+      <c r="C95" s="23"/>
+      <c r="D95" s="23"/>
+      <c r="E95" s="23"/>
+      <c r="F95" s="23"/>
+      <c r="G95" s="23"/>
+      <c r="H95" s="23"/>
+      <c r="I95" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="B10:I10"/>
-    <mergeCell ref="B17:I17"/>
-    <mergeCell ref="B23:I23"/>
-    <mergeCell ref="B44:I44"/>
-    <mergeCell ref="B47:I47"/>
-    <mergeCell ref="B28:I28"/>
-    <mergeCell ref="B16:I16"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B20:I20"/>
-    <mergeCell ref="B26:I26"/>
-    <mergeCell ref="B14:I14"/>
-    <mergeCell ref="B50:I50"/>
-    <mergeCell ref="B29:I29"/>
-    <mergeCell ref="B38:I38"/>
-    <mergeCell ref="B41:I41"/>
-    <mergeCell ref="B32:I32"/>
-    <mergeCell ref="B34:I34"/>
-    <mergeCell ref="B35:I35"/>
+    <mergeCell ref="B92:I92"/>
+    <mergeCell ref="B94:I94"/>
+    <mergeCell ref="B95:I95"/>
+    <mergeCell ref="B89:I89"/>
+    <mergeCell ref="B64:I64"/>
+    <mergeCell ref="B52:I52"/>
+    <mergeCell ref="B58:I58"/>
+    <mergeCell ref="B82:I82"/>
+    <mergeCell ref="B70:I70"/>
+    <mergeCell ref="B76:I76"/>
+    <mergeCell ref="B68:I68"/>
+    <mergeCell ref="B53:I53"/>
+    <mergeCell ref="B56:I56"/>
+    <mergeCell ref="B59:I59"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B5:G5"/>
@@ -2902,20 +2915,24 @@
     <mergeCell ref="B77:I77"/>
     <mergeCell ref="B62:I62"/>
     <mergeCell ref="B65:I65"/>
-    <mergeCell ref="B52:I52"/>
-    <mergeCell ref="B58:I58"/>
-    <mergeCell ref="B82:I82"/>
-    <mergeCell ref="B70:I70"/>
-    <mergeCell ref="B76:I76"/>
-    <mergeCell ref="B68:I68"/>
-    <mergeCell ref="B53:I53"/>
-    <mergeCell ref="B56:I56"/>
-    <mergeCell ref="B59:I59"/>
-    <mergeCell ref="B92:I92"/>
-    <mergeCell ref="B94:I94"/>
-    <mergeCell ref="B95:I95"/>
-    <mergeCell ref="B89:I89"/>
-    <mergeCell ref="B64:I64"/>
+    <mergeCell ref="B50:I50"/>
+    <mergeCell ref="B29:I29"/>
+    <mergeCell ref="B38:I38"/>
+    <mergeCell ref="B41:I41"/>
+    <mergeCell ref="B32:I32"/>
+    <mergeCell ref="B34:I34"/>
+    <mergeCell ref="B35:I35"/>
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B17:I17"/>
+    <mergeCell ref="B23:I23"/>
+    <mergeCell ref="B44:I44"/>
+    <mergeCell ref="B47:I47"/>
+    <mergeCell ref="B28:I28"/>
+    <mergeCell ref="B16:I16"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="B26:I26"/>
+    <mergeCell ref="B14:I14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>